<commit_message>
Faz estimativa atualizada do indicador 4.3.2 (taxa de conclusão ensino superior), renomeia os indicadores que eram 4.3.2 para 4.1.2 e ajusta tratamento da PNAD e subsitui uso de pacotes que requerem Java
</commit_message>
<xml_diff>
--- a/outputs/mvp/ind_4_3_2/ind_4_3_2.xlsx
+++ b/outputs/mvp/ind_4_3_2/ind_4_3_2.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,7 +365,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>n_em_comp</t>
+          <t>n_es_comp</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -401,13 +401,13 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.5205087852764995</v>
+        <v>0.1157449597071815</v>
       </c>
       <c r="C2">
-        <v>0.5110617256502583</v>
+        <v>0.110659413866707</v>
       </c>
       <c r="D2">
-        <v>0.5299558449027406</v>
+        <v>0.1208305055476561</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -432,13 +432,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.5883299441743078</v>
+        <v>0.1372450440773866</v>
       </c>
       <c r="C3">
-        <v>0.5753533145660437</v>
+        <v>0.1306143353250568</v>
       </c>
       <c r="D3">
-        <v>0.601306573782572</v>
+        <v>0.1438757528297164</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -463,13 +463,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.4534537152547192</v>
+        <v>0.09478611450670694</v>
       </c>
       <c r="C4">
-        <v>0.4409321149952654</v>
+        <v>0.08964517299269689</v>
       </c>
       <c r="D4">
-        <v>0.465975315514173</v>
+        <v>0.099927056020717</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.6798862771086508</v>
+        <v>0.3894992841398432</v>
       </c>
       <c r="C5">
-        <v>0.5373143926147207</v>
+        <v>0.2734820122163844</v>
       </c>
       <c r="D5">
-        <v>0.8224581616025809</v>
+        <v>0.5055165560633021</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -525,13 +525,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.6223239538338845</v>
+        <v>0.1901133911758598</v>
       </c>
       <c r="C6">
-        <v>0.6077809971744327</v>
+        <v>0.1806411020195405</v>
       </c>
       <c r="D6">
-        <v>0.6368669104933363</v>
+        <v>0.199585680332179</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -556,13 +556,13 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.3520188917125413</v>
+        <v>0.0260320982038928</v>
       </c>
       <c r="C7">
-        <v>0.1846011071454004</v>
+        <v>-0.00054578193031736</v>
       </c>
       <c r="D7">
-        <v>0.5194366762796822</v>
+        <v>0.05260997833810296</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -587,13 +587,13 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.4481207238795061</v>
+        <v>0.06333074956543937</v>
       </c>
       <c r="C8">
-        <v>0.4361849845669114</v>
+        <v>0.05976251662622011</v>
       </c>
       <c r="D8">
-        <v>0.4600564631921008</v>
+        <v>0.06689898250465863</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -618,13 +618,13 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.5509949179998642</v>
+        <v>0.1315662423217946</v>
       </c>
       <c r="C9">
-        <v>0.5401075925494202</v>
+        <v>0.1256004365954391</v>
       </c>
       <c r="D9">
-        <v>0.5618822434503082</v>
+        <v>0.13753204804815</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -649,13 +649,13 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.3475873823707933</v>
+        <v>0.02614968673508461</v>
       </c>
       <c r="C10">
-        <v>0.3313172148423087</v>
+        <v>0.02271609467075205</v>
       </c>
       <c r="D10">
-        <v>0.3638575498992779</v>
+        <v>0.02958327879941716</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -680,13 +680,13 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.7525013566635764</v>
+        <v>0.3987302775051745</v>
       </c>
       <c r="C11">
-        <v>0.5979855974505246</v>
+        <v>0.2627259259517625</v>
       </c>
       <c r="D11">
-        <v>0.9070171158766283</v>
+        <v>0.5347346290585864</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -711,13 +711,13 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.5483403658183601</v>
+        <v>0.3796609269022687</v>
       </c>
       <c r="C12">
-        <v>0.2299822033785442</v>
+        <v>0.1820641155818325</v>
       </c>
       <c r="D12">
-        <v>0.8666985282581759</v>
+        <v>0.5772577382227049</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -742,13 +742,13 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.6850802185260806</v>
+        <v>0.2173422915613571</v>
       </c>
       <c r="C13">
-        <v>0.6671824905959103</v>
+        <v>0.2049504836477314</v>
       </c>
       <c r="D13">
-        <v>0.7029779464562509</v>
+        <v>0.2297340994749828</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -773,13 +773,13 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.5592500740920143</v>
+        <v>0.1628166526771549</v>
       </c>
       <c r="C14">
-        <v>0.5386811731495675</v>
+        <v>0.1531867194973294</v>
       </c>
       <c r="D14">
-        <v>0.5798189750344611</v>
+        <v>0.1724465858569804</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.3677729154945657</v>
+        <v>0.03200937048174561</v>
       </c>
       <c r="C15">
-        <v>0.1758405260330925</v>
+        <v>-0.009002776101157857</v>
       </c>
       <c r="D15">
-        <v>0.559705304956039</v>
+        <v>0.07302151706464907</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -835,13 +835,13 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.3270061505117726</v>
+        <v>0.01906763438112593</v>
       </c>
       <c r="C16">
-        <v>-0.004292409518898366</v>
+        <v>-0.01991183249728236</v>
       </c>
       <c r="D16">
-        <v>0.6583047105424435</v>
+        <v>0.05804710125953422</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -866,13 +866,13 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.51846800529044</v>
+        <v>0.07960969364593273</v>
       </c>
       <c r="C17">
-        <v>0.5021201997607099</v>
+        <v>0.07474728562476175</v>
       </c>
       <c r="D17">
-        <v>0.5348158108201702</v>
+        <v>0.08447210166710371</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -897,13 +897,13 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.3797377090742785</v>
+        <v>0.04778148751321416</v>
       </c>
       <c r="C18">
-        <v>0.3651781707484155</v>
+        <v>0.04355240754114873</v>
       </c>
       <c r="D18">
-        <v>0.3942972474001415</v>
+        <v>0.05201056748527959</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -928,13 +928,13 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.6157991749106153</v>
+        <v>0.1548017318492023</v>
       </c>
       <c r="C19">
-        <v>0.6010441794950067</v>
+        <v>0.147093501528428</v>
       </c>
       <c r="D19">
-        <v>0.630554170326224</v>
+        <v>0.1625099621699766</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -959,13 +959,13 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.4859408716236696</v>
+        <v>0.1087333072749236</v>
       </c>
       <c r="C20">
-        <v>0.4711049573224939</v>
+        <v>0.1026833698643221</v>
       </c>
       <c r="D20">
-        <v>0.5007767859248452</v>
+        <v>0.1147832446855251</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -990,13 +990,13 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.4242107804503377</v>
+        <v>0.03506875292344752</v>
       </c>
       <c r="C21">
-        <v>0.4009348227081566</v>
+        <v>0.03019132304246943</v>
       </c>
       <c r="D21">
-        <v>0.4474867381925187</v>
+        <v>0.03994618280442562</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1021,13 +1021,13 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.2780955710215698</v>
+        <v>0.01784135141598404</v>
       </c>
       <c r="C22">
-        <v>0.2582922560544571</v>
+        <v>0.0145171018614692</v>
       </c>
       <c r="D22">
-        <v>0.2978988859886826</v>
+        <v>0.02116560097049889</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1052,13 +1052,13 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.7066578653220045</v>
+        <v>0.4083582804277107</v>
       </c>
       <c r="C23">
-        <v>0.5597729627032281</v>
+        <v>0.2868787540717435</v>
       </c>
       <c r="D23">
-        <v>0.8535427679407809</v>
+        <v>0.529837806783678</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1083,13 +1083,13 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.643176511677772</v>
+        <v>0.2083973509022076</v>
       </c>
       <c r="C24">
-        <v>0.6276614620260064</v>
+        <v>0.1979189223886778</v>
       </c>
       <c r="D24">
-        <v>0.6586915613295377</v>
+        <v>0.2188757794157374</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1114,13 +1114,13 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.3614596261798138</v>
+        <v>0.03275479744989286</v>
       </c>
       <c r="C25">
-        <v>0.1522169932965007</v>
+        <v>-0.0005471975953506292</v>
       </c>
       <c r="D25">
-        <v>0.5707022590631268</v>
+        <v>0.06605679249513635</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1145,13 +1145,13 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.4803082446243398</v>
+        <v>0.07339762874725939</v>
       </c>
       <c r="C26">
-        <v>0.4666191367178603</v>
+        <v>0.06908845554190042</v>
       </c>
       <c r="D26">
-        <v>0.4939973525308193</v>
+        <v>0.07770680195261835</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1176,13 +1176,13 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.3089810933460345</v>
+        <v>0.07457146389160679</v>
       </c>
       <c r="C27">
-        <v>0.005944435164810746</v>
+        <v>-0.03200399745990483</v>
       </c>
       <c r="D27">
-        <v>0.6120177515272582</v>
+        <v>0.1811469252431184</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1207,13 +1207,13 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.4577370495424496</v>
+        <v>0.04917397368215704</v>
       </c>
       <c r="C28">
-        <v>0.4286125404813741</v>
+        <v>0.04117596940434439</v>
       </c>
       <c r="D28">
-        <v>0.486861558603525</v>
+        <v>0.05717197795996969</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1238,13 +1238,13 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.3104703208391831</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>0.0605607389759098</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>0.5603799027024563</v>
+        <v>0</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1269,13 +1269,13 @@
         </is>
       </c>
       <c r="B30">
-        <v>0.2981854991459357</v>
+        <v>0.01576353644048987</v>
       </c>
       <c r="C30">
-        <v>0.2800861543018485</v>
+        <v>0.01339559604500088</v>
       </c>
       <c r="D30">
-        <v>0.3162848439900229</v>
+        <v>0.01813147683597887</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1300,13 +1300,13 @@
         </is>
       </c>
       <c r="B31">
-        <v>0.7831144786834734</v>
+        <v>0.4189075595735588</v>
       </c>
       <c r="C31">
-        <v>0.623433835405212</v>
+        <v>0.2779723068208202</v>
       </c>
       <c r="D31">
-        <v>0.9427951219617348</v>
+        <v>0.5598428123262973</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1331,13 +1331,13 @@
         </is>
       </c>
       <c r="B32">
-        <v>0.5722184825599702</v>
+        <v>0.3970469808124463</v>
       </c>
       <c r="C32">
-        <v>0.2445917717418613</v>
+        <v>0.1893111205620243</v>
       </c>
       <c r="D32">
-        <v>0.8998451933780791</v>
+        <v>0.6047828410628684</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1362,13 +1362,13 @@
         </is>
       </c>
       <c r="B33">
-        <v>0.7041976929498933</v>
+        <v>0.2368194165768765</v>
       </c>
       <c r="C33">
-        <v>0.6852176242680807</v>
+        <v>0.2232448574078501</v>
       </c>
       <c r="D33">
-        <v>0.7231777616317059</v>
+        <v>0.2503939757459029</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1393,13 +1393,13 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.5814372490169545</v>
+        <v>0.1796961996145243</v>
       </c>
       <c r="C34">
-        <v>0.5591652216767904</v>
+        <v>0.1688903271559285</v>
       </c>
       <c r="D34">
-        <v>0.6037092763571186</v>
+        <v>0.1905020720731201</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1424,13 +1424,13 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.3727749770597136</v>
+        <v>0.04158848071736164</v>
       </c>
       <c r="C35">
-        <v>0.1109150265966106</v>
+        <v>-0.01182378789653367</v>
       </c>
       <c r="D35">
-        <v>0.6346349275228166</v>
+        <v>0.09500074933125695</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1455,13 +1455,13 @@
         </is>
       </c>
       <c r="B36">
-        <v>0.3450949823811365</v>
+        <v>0.02314067333200219</v>
       </c>
       <c r="C36">
-        <v>-0.03905053066148528</v>
+        <v>-0.02489561938979509</v>
       </c>
       <c r="D36">
-        <v>0.7292404954237584</v>
+        <v>0.07117696605379947</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1486,13 +1486,13 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.5473610002997994</v>
+        <v>0.09138371187600788</v>
       </c>
       <c r="C37">
-        <v>0.5284420126487582</v>
+        <v>0.08547986896152523</v>
       </c>
       <c r="D37">
-        <v>0.5662799879508406</v>
+        <v>0.09728755479049053</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1517,13 +1517,13 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.4137383871929612</v>
+        <v>0.05609054221628659</v>
       </c>
       <c r="C38">
-        <v>0.3959901669150178</v>
+        <v>0.05103797477857699</v>
       </c>
       <c r="D38">
-        <v>0.4314866074709046</v>
+        <v>0.06114310965399619</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1548,13 +1548,13 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.3868040158553888</v>
+        <v>0.04351442022500138</v>
       </c>
       <c r="C39">
-        <v>-0.003430661129387225</v>
+        <v>-0.05022357855193436</v>
       </c>
       <c r="D39">
-        <v>0.7770386928401647</v>
+        <v>0.1372524190019371</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1579,13 +1579,13 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.08826527611596932</v>
+        <v>0.1045074853854435</v>
       </c>
       <c r="C40">
-        <v>-0.1851178619451222</v>
+        <v>-0.05174966551219855</v>
       </c>
       <c r="D40">
-        <v>0.3616484141770608</v>
+        <v>0.2607646362830854</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1610,13 +1610,13 @@
         </is>
       </c>
       <c r="B41">
-        <v>0.5296176090026991</v>
+        <v>0.06231318117313905</v>
       </c>
       <c r="C41">
-        <v>0.4885336079558228</v>
+        <v>0.05109230553229847</v>
       </c>
       <c r="D41">
-        <v>0.5707016100495753</v>
+        <v>0.07353405681397963</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1641,13 +1641,13 @@
         </is>
       </c>
       <c r="B42">
-        <v>0.3891877705802944</v>
+        <v>0.03672129571990859</v>
       </c>
       <c r="C42">
-        <v>0.3502670177782404</v>
+        <v>0.02845020957672158</v>
       </c>
       <c r="D42">
-        <v>0.4281085233823483</v>
+        <v>0.0449923818630956</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1672,13 +1672,13 @@
         </is>
       </c>
       <c r="B43">
-        <v>0.349491396821422</v>
+        <v>0</v>
       </c>
       <c r="C43">
-        <v>0.0565583903626336</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>0.6424244032802104</v>
+        <v>0</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1703,13 +1703,13 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.2140419265475456</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <v>-0.1733452719225366</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>0.6014291250176278</v>
+        <v>0</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1734,13 +1734,13 @@
         </is>
       </c>
       <c r="B45">
-        <v>0.3753064940498632</v>
+        <v>0.02275236415265728</v>
       </c>
       <c r="C45">
-        <v>0.346857887220931</v>
+        <v>0.01871295666508674</v>
       </c>
       <c r="D45">
-        <v>0.4037551008787953</v>
+        <v>0.02679177164022781</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1765,13 +1765,13 @@
         </is>
       </c>
       <c r="B46">
-        <v>0.2302439653192013</v>
+        <v>0.009316788866164579</v>
       </c>
       <c r="C46">
-        <v>0.2090676272619472</v>
+        <v>0.006596987395953319</v>
       </c>
       <c r="D46">
-        <v>0.2514203033764554</v>
+        <v>0.01203659033637584</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1796,13 +1796,13 @@
         </is>
       </c>
       <c r="B47">
-        <v>0.6267097335965982</v>
+        <v>0.1525514218328415</v>
       </c>
       <c r="C47">
-        <v>0.6166785200345558</v>
+        <v>0.1472538849347267</v>
       </c>
       <c r="D47">
-        <v>0.6367409471586406</v>
+        <v>0.1578489587309563</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1827,13 +1827,13 @@
         </is>
       </c>
       <c r="B48">
-        <v>0.6803842135301468</v>
+        <v>0.1845769204969594</v>
       </c>
       <c r="C48">
-        <v>0.664701441206159</v>
+        <v>0.1771538257408943</v>
       </c>
       <c r="D48">
-        <v>0.6960669858541345</v>
+        <v>0.1920000152530244</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1858,13 +1858,13 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.5733615695797295</v>
+        <v>0.1219266034326537</v>
       </c>
       <c r="C49">
-        <v>0.5590866792636086</v>
+        <v>0.1160580168397138</v>
       </c>
       <c r="D49">
-        <v>0.5876364598958504</v>
+        <v>0.1277951900255937</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1889,13 +1889,13 @@
         </is>
       </c>
       <c r="B50">
-        <v>0.7819730176321882</v>
+        <v>0.2595112632955417</v>
       </c>
       <c r="C50">
-        <v>0.6812735776325597</v>
+        <v>0.1319195131209235</v>
       </c>
       <c r="D50">
-        <v>0.8826724576318167</v>
+        <v>0.3871030134701601</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1920,13 +1920,13 @@
         </is>
       </c>
       <c r="B51">
-        <v>0.7050111631694674</v>
+        <v>0.2384865360028557</v>
       </c>
       <c r="C51">
-        <v>0.6896078692107845</v>
+        <v>0.2287681790073758</v>
       </c>
       <c r="D51">
-        <v>0.7204144571281503</v>
+        <v>0.2482048929983355</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1951,13 +1951,13 @@
         </is>
       </c>
       <c r="B52">
-        <v>0.8487417668227265</v>
+        <v>0.2919688620359776</v>
       </c>
       <c r="C52">
-        <v>0.3769757197161411</v>
+        <v>-0.01542271583104576</v>
       </c>
       <c r="D52">
-        <v>1.320507813929312</v>
+        <v>0.599360439903001</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1982,13 +1982,13 @@
         </is>
       </c>
       <c r="B53">
-        <v>0.5756515349310275</v>
+        <v>0.070481581039622</v>
       </c>
       <c r="C53">
-        <v>0.4522896520786315</v>
+        <v>0.0316193870061598</v>
       </c>
       <c r="D53">
-        <v>0.6990134177834235</v>
+        <v>0.1093437750730842</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2013,13 +2013,13 @@
         </is>
       </c>
       <c r="B54">
-        <v>0.5754311914996646</v>
+        <v>0.09944431530180564</v>
       </c>
       <c r="C54">
-        <v>0.5620514635617284</v>
+        <v>0.09409017423133405</v>
       </c>
       <c r="D54">
-        <v>0.5888109194376008</v>
+        <v>0.1047984563722772</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2044,13 +2044,13 @@
         </is>
       </c>
       <c r="B55">
-        <v>0.6522965238577458</v>
+        <v>0.1700295179412862</v>
       </c>
       <c r="C55">
-        <v>0.6409774971471741</v>
+        <v>0.1639450609551262</v>
       </c>
       <c r="D55">
-        <v>0.6636155505683176</v>
+        <v>0.1761139749274462</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2075,13 +2075,13 @@
         </is>
       </c>
       <c r="B56">
-        <v>0.4610600202932325</v>
+        <v>0.03909251859034588</v>
       </c>
       <c r="C56">
-        <v>0.4413245760378223</v>
+        <v>0.03489801695916797</v>
       </c>
       <c r="D56">
-        <v>0.4807954645486426</v>
+        <v>0.04328702022152378</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2106,13 +2106,13 @@
         </is>
       </c>
       <c r="B57">
-        <v>0.7854220154893108</v>
+        <v>0.3185362280432101</v>
       </c>
       <c r="C57">
-        <v>0.6636888243051753</v>
+        <v>0.1313076468181143</v>
       </c>
       <c r="D57">
-        <v>0.9071552066734463</v>
+        <v>0.5057648092683059</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2137,13 +2137,13 @@
         </is>
       </c>
       <c r="B58">
-        <v>0.7759205980589818</v>
+        <v>0.176349620963158</v>
       </c>
       <c r="C58">
-        <v>0.6138961935973321</v>
+        <v>0.1017808249215216</v>
       </c>
       <c r="D58">
-        <v>0.9379450025206316</v>
+        <v>0.2509184170047943</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2168,13 +2168,13 @@
         </is>
       </c>
       <c r="B59">
-        <v>0.7459293616478715</v>
+        <v>0.28639255623495</v>
       </c>
       <c r="C59">
-        <v>0.7208585324221655</v>
+        <v>0.2719003191225132</v>
       </c>
       <c r="D59">
-        <v>0.7710001908735775</v>
+        <v>0.3008847933473868</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2199,13 +2199,13 @@
         </is>
       </c>
       <c r="B60">
-        <v>0.6628191285848473</v>
+        <v>0.1928041920705239</v>
       </c>
       <c r="C60">
-        <v>0.640351652935119</v>
+        <v>0.1810137003889488</v>
       </c>
       <c r="D60">
-        <v>0.6852866042345755</v>
+        <v>0.204594683752099</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2230,13 +2230,13 @@
         </is>
       </c>
       <c r="B61">
-        <v>0.8487417668227265</v>
+        <v>0.3236876275885627</v>
       </c>
       <c r="C61">
-        <v>0.3769757197161411</v>
+        <v>-0.03124397796776723</v>
       </c>
       <c r="D61">
-        <v>1.320507813929312</v>
+        <v>0.6786192331448926</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2261,22 +2261,22 @@
         </is>
       </c>
       <c r="B62">
-        <v>0.5627173496012672</v>
+        <v>0.1237109835054415</v>
       </c>
       <c r="C62">
-        <v>0.4017391966856895</v>
+        <v>-0.3250386130940447</v>
       </c>
       <c r="D62">
-        <v>0.7236955025168448</v>
+        <v>0.5724605801049277</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Ignorado</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -2292,17 +2292,17 @@
         </is>
       </c>
       <c r="B63">
-        <v>0.5997363790280306</v>
+        <v>0.1010467449713592</v>
       </c>
       <c r="C63">
-        <v>0.4286267067873478</v>
+        <v>0.03543983503777987</v>
       </c>
       <c r="D63">
-        <v>0.7708460512687133</v>
+        <v>0.1666536549049384</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2323,22 +2323,22 @@
         </is>
       </c>
       <c r="B64">
-        <v>0.6364169108490763</v>
+        <v>0.03149217887208097</v>
       </c>
       <c r="C64">
-        <v>0.6167827705776678</v>
+        <v>0.007817754309228417</v>
       </c>
       <c r="D64">
-        <v>0.6560510511204847</v>
+        <v>0.05516660343493351</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -2354,17 +2354,17 @@
         </is>
       </c>
       <c r="B65">
-        <v>0.5168680144727671</v>
+        <v>0.1210463729950209</v>
       </c>
       <c r="C65">
-        <v>0.4985034342126638</v>
+        <v>0.1134898876377366</v>
       </c>
       <c r="D65">
-        <v>0.5352325947328703</v>
+        <v>0.1286028583523051</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2385,27 +2385,27 @@
         </is>
       </c>
       <c r="B66">
-        <v>0.6985762325791974</v>
+        <v>0.07892011053617835</v>
       </c>
       <c r="C66">
-        <v>0.6816129472813962</v>
+        <v>0.07299741635872381</v>
       </c>
       <c r="D66">
-        <v>0.7155395178769987</v>
+        <v>0.0848428047136329</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Total</t>
         </is>
       </c>
     </row>
@@ -2416,17 +2416,17 @@
         </is>
       </c>
       <c r="B67">
-        <v>0.6055995434701777</v>
+        <v>0.2046681212225473</v>
       </c>
       <c r="C67">
-        <v>0.590059128593057</v>
+        <v>0.196244840755158</v>
       </c>
       <c r="D67">
-        <v>0.6211399583472985</v>
+        <v>0.2130914016899367</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -2447,17 +2447,17 @@
         </is>
       </c>
       <c r="B68">
-        <v>0.5556112530846508</v>
+        <v>0.1367044347362849</v>
       </c>
       <c r="C68">
-        <v>0.5279033599855727</v>
+        <v>0.1299822136637989</v>
       </c>
       <c r="D68">
-        <v>0.5833191461837288</v>
+        <v>0.1434266558087708</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -2478,17 +2478,17 @@
         </is>
       </c>
       <c r="B69">
-        <v>0.375829315421558</v>
+        <v>0.05106438800066936</v>
       </c>
       <c r="C69">
-        <v>0.3477532115875966</v>
+        <v>0.0453879005039946</v>
       </c>
       <c r="D69">
-        <v>0.4039054192555193</v>
+        <v>0.05674087549734411</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -2509,27 +2509,27 @@
         </is>
       </c>
       <c r="B70">
-        <v>0.808943808869894</v>
+        <v>0.02808637851507721</v>
       </c>
       <c r="C70">
-        <v>0.7004802015244317</v>
+        <v>0.02191522773435541</v>
       </c>
       <c r="D70">
-        <v>0.9174074162153564</v>
+        <v>0.03425752929579901</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
@@ -2540,13 +2540,13 @@
         </is>
       </c>
       <c r="B71">
-        <v>0.7207308766129847</v>
+        <v>0.276366228551203</v>
       </c>
       <c r="C71">
-        <v>0.7039309261246653</v>
+        <v>0.1371048521220302</v>
       </c>
       <c r="D71">
-        <v>0.7375308271013041</v>
+        <v>0.4156276049803759</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2555,7 +2555,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -2571,13 +2571,13 @@
         </is>
       </c>
       <c r="B72">
-        <v>0.8487417668227265</v>
+        <v>0.2572860609028331</v>
       </c>
       <c r="C72">
-        <v>0.3769757197161411</v>
+        <v>0.2466471601914433</v>
       </c>
       <c r="D72">
-        <v>1.320507813929312</v>
+        <v>0.2679249616142229</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Ignorado</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -2602,13 +2602,13 @@
         </is>
       </c>
       <c r="B73">
-        <v>0.5656837758972229</v>
+        <v>0.2998061235770649</v>
       </c>
       <c r="C73">
-        <v>0.42011087392321</v>
+        <v>-0.01476039645761551</v>
       </c>
       <c r="D73">
-        <v>0.7112566778712357</v>
+        <v>0.6143726436117454</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Ignorado</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -2633,13 +2633,13 @@
         </is>
       </c>
       <c r="B74">
-        <v>0.6044021102821973</v>
+        <v>0.08355207802668148</v>
       </c>
       <c r="C74">
-        <v>0.588911641072898</v>
+        <v>0.03548093139414821</v>
       </c>
       <c r="D74">
-        <v>0.6198925794914966</v>
+        <v>0.1316232246592147</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -2664,13 +2664,13 @@
         </is>
       </c>
       <c r="B75">
-        <v>0.5843896021854414</v>
+        <v>0.1127235347075406</v>
       </c>
       <c r="C75">
-        <v>0.3202752462035586</v>
+        <v>0.1064092303668353</v>
       </c>
       <c r="D75">
-        <v>0.8485039581673244</v>
+        <v>0.1190378390482459</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2679,12 +2679,12 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -2695,13 +2695,13 @@
         </is>
       </c>
       <c r="B76">
-        <v>0.5610168308940722</v>
+        <v>0.1057969117123234</v>
       </c>
       <c r="C76">
-        <v>0.5266747776495031</v>
+        <v>-0.01034609049822276</v>
       </c>
       <c r="D76">
-        <v>0.5953588841386412</v>
+        <v>0.2219399139228695</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2710,7 +2710,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -2726,13 +2726,13 @@
         </is>
       </c>
       <c r="B77">
-        <v>0.6133578450327439</v>
+        <v>0.07051918527058711</v>
       </c>
       <c r="C77">
-        <v>0.4073307901205955</v>
+        <v>0.06076735321534283</v>
       </c>
       <c r="D77">
-        <v>0.8193848999448924</v>
+        <v>0.08027101732583138</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -2757,13 +2757,13 @@
         </is>
       </c>
       <c r="B78">
-        <v>0.4187975307593188</v>
+        <v>0</v>
       </c>
       <c r="C78">
-        <v>0.395162644343618</v>
+        <v>0</v>
       </c>
       <c r="D78">
-        <v>0.4424324171750196</v>
+        <v>0</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2772,7 +2772,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Ignorado</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -2788,27 +2788,27 @@
         </is>
       </c>
       <c r="B79">
-        <v>0.8016680713086706</v>
+        <v>0.008942918134920477</v>
       </c>
       <c r="C79">
-        <v>0.6684043828234163</v>
+        <v>-0.005018366013423937</v>
       </c>
       <c r="D79">
-        <v>0.9349317597939248</v>
+        <v>0.02290420228326489</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
@@ -2819,27 +2819,27 @@
         </is>
       </c>
       <c r="B80">
-        <v>0.8215041096551486</v>
+        <v>0.02629568476344547</v>
       </c>
       <c r="C80">
-        <v>0.6588214644051604</v>
+        <v>0.02199755131399797</v>
       </c>
       <c r="D80">
-        <v>0.9841867549051369</v>
+        <v>0.03059381821289298</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
@@ -2850,13 +2850,13 @@
         </is>
       </c>
       <c r="B81">
-        <v>0.755231814389237</v>
+        <v>0.3318192936475043</v>
       </c>
       <c r="C81">
-        <v>0.7282074883779392</v>
+        <v>0.1305866766577099</v>
       </c>
       <c r="D81">
-        <v>0.7822561404005348</v>
+        <v>0.5330519106372987</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2865,7 +2865,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -2881,13 +2881,13 @@
         </is>
       </c>
       <c r="B82">
-        <v>0.6848286877265829</v>
+        <v>0.1953698655884353</v>
       </c>
       <c r="C82">
-        <v>0.6607546999904412</v>
+        <v>0.1125721946107827</v>
       </c>
       <c r="D82">
-        <v>0.7089026754627246</v>
+        <v>0.2781675365660878</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -2912,13 +2912,13 @@
         </is>
       </c>
       <c r="B83">
-        <v>0.8487417668227265</v>
+        <v>0.3070666041964848</v>
       </c>
       <c r="C83">
-        <v>0.3769757197161411</v>
+        <v>0.2914414448968591</v>
       </c>
       <c r="D83">
-        <v>1.320507813929312</v>
+        <v>0.3226917634961106</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Ignorado</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -2943,22 +2943,22 @@
         </is>
       </c>
       <c r="B84">
-        <v>0.5458361498483792</v>
+        <v>0.2094737045567619</v>
       </c>
       <c r="C84">
-        <v>0.3624121702430718</v>
+        <v>0.1964396097571276</v>
       </c>
       <c r="D84">
-        <v>0.7292601294536867</v>
+        <v>0.2225077993563962</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -2974,22 +2974,22 @@
         </is>
       </c>
       <c r="B85">
-        <v>0.6137386433401236</v>
+        <v>0.3236876275885627</v>
       </c>
       <c r="C85">
-        <v>0.4125977174767913</v>
+        <v>-0.03124397796776723</v>
       </c>
       <c r="D85">
-        <v>0.8148795692034559</v>
+        <v>0.6786192331448926</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Ignorado</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -3005,22 +3005,22 @@
         </is>
       </c>
       <c r="B86">
-        <v>0.6583281186406126</v>
+        <v>0.1481233826025561</v>
       </c>
       <c r="C86">
-        <v>0.6367483089477953</v>
+        <v>-0.407519685048721</v>
       </c>
       <c r="D86">
-        <v>0.6799079283334298</v>
+        <v>0.7037664502538332</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Ignorado</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -3036,22 +3036,22 @@
         </is>
       </c>
       <c r="B87">
-        <v>0.5517653207895646</v>
+        <v>0.1167497955678974</v>
       </c>
       <c r="C87">
-        <v>0.5311310477981909</v>
+        <v>0.03934641856262165</v>
       </c>
       <c r="D87">
-        <v>0.5723995937809384</v>
+        <v>0.1941531725731731</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -3067,27 +3067,27 @@
         </is>
       </c>
       <c r="B88">
-        <v>0.6720636351116106</v>
+        <v>0.03741296048461659</v>
       </c>
       <c r="C88">
-        <v>0.3814651939582906</v>
+        <v>0.007806353860538753</v>
       </c>
       <c r="D88">
-        <v>0.9626620762649305</v>
+        <v>0.06701956710869442</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -3098,27 +3098,27 @@
         </is>
       </c>
       <c r="B89">
-        <v>0.410500046859641</v>
+        <v>0.1367613135295222</v>
       </c>
       <c r="C89">
-        <v>-0.1103139581951066</v>
+        <v>0.1279464778345429</v>
       </c>
       <c r="D89">
-        <v>0.9313140519143885</v>
+        <v>0.1455761492245015</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -3129,27 +3129,27 @@
         </is>
       </c>
       <c r="B90">
-        <v>0.6566477554674751</v>
+        <v>0.08979431075952357</v>
       </c>
       <c r="C90">
-        <v>0.6096505445008983</v>
+        <v>0.08290017516602249</v>
       </c>
       <c r="D90">
-        <v>0.7036449664340519</v>
+        <v>0.09668844635302465</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -3160,22 +3160,22 @@
         </is>
       </c>
       <c r="B91">
-        <v>0.470340068366966</v>
+        <v>0.1762348323952785</v>
       </c>
       <c r="C91">
-        <v>0.4219755644163128</v>
+        <v>-0.03472981483342744</v>
       </c>
       <c r="D91">
-        <v>0.5187045723176192</v>
+        <v>0.3871994796239844</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -3191,22 +3191,22 @@
         </is>
       </c>
       <c r="B92">
-        <v>0.6667003505193594</v>
+        <v>0.03384293903201641</v>
       </c>
       <c r="C92">
-        <v>0.3395662789258327</v>
+        <v>-0.04027012312141521</v>
       </c>
       <c r="D92">
-        <v>0.9938344221128861</v>
+        <v>0.107956001185448</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -3222,22 +3222,22 @@
         </is>
       </c>
       <c r="B93">
-        <v>0.5723523885987959</v>
+        <v>0.09469367258487407</v>
       </c>
       <c r="C93">
-        <v>0.2446156674717931</v>
+        <v>0.07947495610088456</v>
       </c>
       <c r="D93">
-        <v>0.9000891097257987</v>
+        <v>0.1099123890688636</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -3253,22 +3253,22 @@
         </is>
       </c>
       <c r="B94">
-        <v>0.5113279911638051</v>
+        <v>0.04890263904440549</v>
       </c>
       <c r="C94">
-        <v>0.4762838724222757</v>
+        <v>0.03872960065079427</v>
       </c>
       <c r="D94">
-        <v>0.5463721099053346</v>
+        <v>0.05907567743801671</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -3284,13 +3284,13 @@
         </is>
       </c>
       <c r="B95">
-        <v>0.3374660754619274</v>
+        <v>0</v>
       </c>
       <c r="C95">
-        <v>0.3048793762533923</v>
+        <v>0</v>
       </c>
       <c r="D95">
-        <v>0.3700527746704624</v>
+        <v>0</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3299,10 +3299,134 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B96">
+        <v>0.007915871588281904</v>
+      </c>
+      <c r="C96">
+        <v>-0.008278312603163682</v>
+      </c>
+      <c r="D96">
+        <v>0.02411005577972749</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B97">
+        <v>0.009823743962719062</v>
+      </c>
+      <c r="C97">
+        <v>-0.01133884582795784</v>
+      </c>
+      <c r="D97">
+        <v>0.03098633375339597</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B98">
+        <v>0.033320740084171</v>
+      </c>
+      <c r="C98">
+        <v>0.02829884793796158</v>
+      </c>
+      <c r="D98">
+        <v>0.03834263223038042</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
           <t>Preto ou pardo</t>
         </is>
       </c>
-      <c r="G95" t="inlineStr">
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B99">
+        <v>0.01976555397769849</v>
+      </c>
+      <c r="C99">
+        <v>0.0123334074457472</v>
+      </c>
+      <c r="D99">
+        <v>0.02719770050964979</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
         <is>
           <t>Rural</t>
         </is>

</xml_diff>